<commit_message>
estimate of indrayani mandir signed and estimate of gravel in pashikhel bhitri baato given along with jasta tahara naksha field measurement
</commit_message>
<xml_diff>
--- a/ofc/estimates/bhaipari/pashikhel gravel baato.xlsx
+++ b/ofc/estimates/bhaipari/pashikhel gravel baato.xlsx
@@ -47,6 +47,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Estimate!$A$1:$K$78</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">final!$A$1:$K$60</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Sheet4 (2)'!$A$1:$K$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">ग्रावेल!$A$1:$K$28</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Estimate!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">final!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'Sheet4 (2)'!$1:$8</definedName>
@@ -821,17 +822,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -846,30 +849,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -889,6 +875,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1559,38 +1560,38 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="110" t="s">
+      <c r="H7" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3239,11 +3240,11 @@
       <c r="B73" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="112">
+      <c r="C73" s="110">
         <f>J71</f>
         <v>1194331.7948368895</v>
       </c>
-      <c r="D73" s="113"/>
+      <c r="D73" s="111"/>
       <c r="E73" s="16">
         <v>100</v>
       </c>
@@ -3258,21 +3259,21 @@
       <c r="B74" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="119">
+      <c r="C74" s="112">
         <v>1000000</v>
       </c>
-      <c r="D74" s="120"/>
+      <c r="D74" s="113"/>
       <c r="E74" s="16"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C75" s="119">
+      <c r="C75" s="112">
         <f>C74-C77-C78</f>
         <v>950000</v>
       </c>
-      <c r="D75" s="120"/>
+      <c r="D75" s="113"/>
       <c r="E75" s="16">
         <f>C75/C73*100</f>
         <v>79.542385466656867</v>
@@ -3282,11 +3283,11 @@
       <c r="B76" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="118">
+      <c r="C76" s="109">
         <f>C73-C75</f>
         <v>244331.79483688949</v>
       </c>
-      <c r="D76" s="118"/>
+      <c r="D76" s="109"/>
       <c r="E76" s="16">
         <f>100-E75</f>
         <v>20.457614533343133</v>
@@ -3296,11 +3297,11 @@
       <c r="B77" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C77" s="112">
+      <c r="C77" s="110">
         <f>C74*0.03</f>
         <v>30000</v>
       </c>
-      <c r="D77" s="113"/>
+      <c r="D77" s="111"/>
       <c r="E77" s="16">
         <v>3</v>
       </c>
@@ -3309,32 +3310,32 @@
       <c r="B78" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="112">
+      <c r="C78" s="110">
         <f>C74*0.02</f>
         <v>20000</v>
       </c>
-      <c r="D78" s="113"/>
+      <c r="D78" s="111"/>
       <c r="E78" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C73:D73"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3448,38 +3449,38 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="110" t="s">
+      <c r="H7" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -4644,11 +4645,11 @@
       <c r="B55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="112">
+      <c r="C55" s="110">
         <f>J53</f>
         <v>563311.92829411826</v>
       </c>
-      <c r="D55" s="113"/>
+      <c r="D55" s="111"/>
       <c r="E55" s="16">
         <v>100</v>
       </c>
@@ -4664,10 +4665,10 @@
       <c r="B56" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="119">
+      <c r="C56" s="112">
         <v>500000</v>
       </c>
-      <c r="D56" s="120"/>
+      <c r="D56" s="113"/>
       <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -4675,11 +4676,11 @@
       <c r="B57" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="119">
+      <c r="C57" s="112">
         <f>C56-C59-C60</f>
         <v>475000</v>
       </c>
-      <c r="D57" s="120"/>
+      <c r="D57" s="113"/>
       <c r="E57" s="16">
         <f>C57/C55*100</f>
         <v>84.322730647377924</v>
@@ -4690,11 +4691,11 @@
       <c r="B58" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="118">
+      <c r="C58" s="109">
         <f>C55-C57</f>
         <v>88311.928294118261</v>
       </c>
-      <c r="D58" s="118"/>
+      <c r="D58" s="109"/>
       <c r="E58" s="16">
         <f>100-E57</f>
         <v>15.677269352622076</v>
@@ -4705,11 +4706,11 @@
       <c r="B59" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="112">
+      <c r="C59" s="110">
         <f>C56*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D59" s="113"/>
+      <c r="D59" s="111"/>
       <c r="E59" s="16">
         <v>3</v>
       </c>
@@ -4719,24 +4720,17 @@
       <c r="B60" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="112">
+      <c r="C60" s="110">
         <f>C56*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D60" s="113"/>
+      <c r="D60" s="111"/>
       <c r="E60" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="A7:F7"/>
@@ -4745,6 +4739,13 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4785,34 +4786,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="116" t="s">
@@ -4845,30 +4846,30 @@
       <c r="K4" s="116"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
+      <c r="K5" s="132"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="121" t="e">
+      <c r="C6" s="128" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="122"/>
+      <c r="D6" s="129"/>
       <c r="E6" s="13"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4876,11 +4877,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="121" t="e">
+      <c r="J6" s="128" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="122"/>
+      <c r="K6" s="129"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
@@ -4889,77 +4890,77 @@
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="I7" s="129" t="s">
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="I7" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="109" t="str">
+      <c r="A8" s="118" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बेन्डोल हाईट सडक निर्माण</v>
       </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="I8" s="130" t="s">
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="I8" s="125" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="130"/>
-      <c r="K8" s="130"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="125"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="131" t="str">
+      <c r="A9" s="126" t="str">
         <f>Estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-      <c r="I9" s="130" t="s">
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="I9" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="125"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="126" t="s">
+      <c r="A11" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="D11" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132" t="s">
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="126" t="s">
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="127" t="s">
+      <c r="K11" s="122" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="126"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="126"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
@@ -4978,8 +4979,8 @@
       <c r="I12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="126"/>
-      <c r="K12" s="127"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="122"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
@@ -5141,6 +5142,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -5154,13 +5162,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5272,21 +5273,21 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="133" t="s">
@@ -6448,10 +6449,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S85"/>
+  <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:K4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,21 +6545,21 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="133" t="s">
@@ -6641,15 +6642,15 @@
         <v>80</v>
       </c>
       <c r="E10" s="78">
-        <f>8/3.281</f>
-        <v>2.4382810118866196</v>
+        <f>(8-2)/3.281</f>
+        <v>1.8287107589149649</v>
       </c>
       <c r="F10" s="78">
         <v>0.15</v>
       </c>
       <c r="G10" s="79">
         <f>PRODUCT(C10:F10)</f>
-        <v>29.259372142639435</v>
+        <v>21.944529106979576</v>
       </c>
       <c r="H10" s="80"/>
       <c r="I10" s="80"/>
@@ -6674,7 +6675,7 @@
       <c r="F11" s="32"/>
       <c r="G11" s="34">
         <f>SUM(G10:G10)</f>
-        <v>29.259372142639435</v>
+        <v>21.944529106979576</v>
       </c>
       <c r="H11" s="33" t="s">
         <v>29</v>
@@ -6684,7 +6685,7 @@
       </c>
       <c r="J11" s="81">
         <f>G11*I11</f>
-        <v>1891.0332215787867</v>
+        <v>1418.27491618409</v>
       </c>
       <c r="K11" s="32"/>
       <c r="M11" s="36"/>
@@ -6709,7 +6710,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="81">
         <f>0.13*G11*19284/360</f>
-        <v>203.75251447729349</v>
+        <v>152.81438585797014</v>
       </c>
       <c r="K12" s="32"/>
       <c r="M12" s="36"/>
@@ -6778,7 +6779,7 @@
       </c>
       <c r="E15" s="78">
         <f>E10</f>
-        <v>2.4382810118866196</v>
+        <v>1.8287107589149649</v>
       </c>
       <c r="F15" s="78">
         <f>F10</f>
@@ -6786,7 +6787,7 @@
       </c>
       <c r="G15" s="79">
         <f>PRODUCT(C15:F15)</f>
-        <v>29.259372142639435</v>
+        <v>21.944529106979576</v>
       </c>
       <c r="H15" s="80"/>
       <c r="I15" s="80"/>
@@ -6820,7 +6821,7 @@
       <c r="F16" s="78"/>
       <c r="G16" s="59">
         <f>SUM(G15:G15)</f>
-        <v>29.259372142639435</v>
+        <v>21.944529106979576</v>
       </c>
       <c r="H16" s="80" t="s">
         <v>29</v>
@@ -6829,9 +6830,9 @@
         <f>1693.85</f>
         <v>1693.85</v>
       </c>
-      <c r="J16" s="80">
+      <c r="J16" s="81">
         <f>G16*I16</f>
-        <v>49560.987503809803</v>
+        <v>37170.740627857354</v>
       </c>
       <c r="K16" s="32"/>
       <c r="M16" s="36"/>
@@ -6857,9 +6858,9 @@
       <c r="G17" s="81"/>
       <c r="H17" s="80"/>
       <c r="I17" s="80"/>
-      <c r="J17" s="80">
+      <c r="J17" s="81">
         <f>0.13*G16*(446551.8+48114)/300</f>
-        <v>6271.8979823224618</v>
+        <v>4703.9234867418463</v>
       </c>
       <c r="K17" s="32"/>
       <c r="M17" s="36"/>
@@ -6960,7 +6961,7 @@
       <c r="I21" s="81"/>
       <c r="J21" s="81">
         <f>SUM(J11:J19)</f>
-        <v>58427.67122218835</v>
+        <v>43945.753416641266</v>
       </c>
       <c r="K21" s="76"/>
     </row>
@@ -6984,7 +6985,7 @@
       </c>
       <c r="C23" s="135">
         <f>J21</f>
-        <v>58427.67122218835</v>
+        <v>43945.753416641266</v>
       </c>
       <c r="D23" s="135"/>
       <c r="E23" s="79">
@@ -7003,7 +7004,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="136">
-        <v>50000</v>
+        <v>35000</v>
       </c>
       <c r="D24" s="136"/>
       <c r="E24" s="79"/>
@@ -7021,12 +7022,12 @@
       </c>
       <c r="C25" s="136">
         <f>C24-C27-C28</f>
-        <v>47500</v>
+        <v>33250</v>
       </c>
       <c r="D25" s="136"/>
       <c r="E25" s="79">
         <f>C25/C23*100</f>
-        <v>81.297096061500255</v>
+        <v>75.661463087828125</v>
       </c>
       <c r="F25" s="90"/>
       <c r="G25" s="89"/>
@@ -7042,12 +7043,12 @@
       </c>
       <c r="C26" s="135">
         <f>C23-C25</f>
-        <v>10927.67122218835</v>
+        <v>10695.753416641266</v>
       </c>
       <c r="D26" s="135"/>
       <c r="E26" s="79">
         <f>100-E25</f>
-        <v>18.702903938499745</v>
+        <v>24.338536912171875</v>
       </c>
       <c r="F26" s="90"/>
       <c r="G26" s="89"/>
@@ -7063,7 +7064,7 @@
       </c>
       <c r="C27" s="135">
         <f>C24*0.03</f>
-        <v>1500</v>
+        <v>1050</v>
       </c>
       <c r="D27" s="135"/>
       <c r="E27" s="79">
@@ -7083,7 +7084,7 @@
       </c>
       <c r="C28" s="135">
         <f>C24*0.02</f>
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="D28" s="135"/>
       <c r="E28" s="79">
@@ -7159,21 +7160,8 @@
     <row r="77" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="78" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="79" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="A7:F7"/>
@@ -7182,9 +7170,16 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>
@@ -7289,21 +7284,21 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="133" t="s">
@@ -8620,6 +8615,13 @@
     <row r="113" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="A7:F7"/>
@@ -8628,13 +8630,6 @@
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8645,7 +8640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S109"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
@@ -8739,21 +8734,21 @@
       <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="133" t="s">
@@ -9948,6 +9943,13 @@
     <row r="109" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="A7:F7"/>
@@ -9956,13 +9958,6 @@
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>